<commit_message>
bug fix lookup options
</commit_message>
<xml_diff>
--- a/src/main/resources/workbooks/TestSet1.xlsx
+++ b/src/main/resources/workbooks/TestSet1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmcmaster/Workspace/scm/xlsx-lookup/src/test/resources/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmcmaster/Workspace/scm/xlsx-lookup/src/main/resources/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31620" windowHeight="19560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31620" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="7" r:id="rId1"/>
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,7 +1697,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1857,7 +1857,7 @@
   <dimension ref="C2:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2287,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>